<commit_message>
Adds specification list for LOS extension exercise 2
</commit_message>
<xml_diff>
--- a/LOS_Anforderungsliste.xlsx
+++ b/LOS_Anforderungsliste.xlsx
@@ -4,22 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="18915" windowHeight="8505"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="18915" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="Aufgabe1" sheetId="1" r:id="rId1"/>
+    <sheet name="Aufgabe2" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$D$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Aufgabe1!$A$1:$D$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Aufgabe2!$A$1:$D$32</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="82">
   <si>
     <t>Nr.</t>
   </si>
@@ -166,6 +166,105 @@
   </si>
   <si>
     <t>(Passed)</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>Attributsdeklarationen dürfen nicht überschrieben werden</t>
+  </si>
+  <si>
+    <t>Methoden</t>
+  </si>
+  <si>
+    <t>Super</t>
+  </si>
+  <si>
+    <t>Aufzählungstypen</t>
+  </si>
+  <si>
+    <t>mit Enum werden global deklariert</t>
+  </si>
+  <si>
+    <t>keine leere Tabelle</t>
+  </si>
+  <si>
+    <t>Die Namen und die Werte dürfen keine leere String oder leere Zeichen enthalten.</t>
+  </si>
+  <si>
+    <t>Mehrere Werte des gleichen Namens sind nicht erlaubt.</t>
+  </si>
+  <si>
+    <t>Bei der Instanziierung eines Objekts, wird mit dem default-Wert initialisiert.</t>
+  </si>
+  <si>
+    <t>Methoden der Oberklasse dürfen überschrieben werden</t>
+  </si>
+  <si>
+    <t>Konstruktoren der Oberklasse dürfen überschrieben werden</t>
+  </si>
+  <si>
+    <t>Aufrufe eine Methode der Oberklasse ist möglich mit super:...()</t>
+  </si>
+  <si>
+    <t>"super" innerhalb von create-Methoden (und nur dort) auch überschriebene Konstruktoren aufgerufen werden können</t>
+  </si>
+  <si>
+    <t>Fehlermeldung bei Verwendung ausserhalb einer Methode</t>
+  </si>
+  <si>
+    <t>default: wenn die Wert leer ist dann der erste Wert nehmen wir als Default</t>
+  </si>
+  <si>
+    <t>Polymorphie soll unterstützt werden</t>
+  </si>
+  <si>
+    <t>Vererbung</t>
+  </si>
+  <si>
+    <t>Es soll möglich sein eine Klasse von einer anderen Klasse abzuleiten. Dabei sollen Methoden und Attribute geerbt werden</t>
+  </si>
+  <si>
+    <t>1.1.</t>
+  </si>
+  <si>
+    <t>3.1.</t>
+  </si>
+  <si>
+    <t>2.1.</t>
+  </si>
+  <si>
+    <t>2.2.</t>
+  </si>
+  <si>
+    <t>3.2.</t>
+  </si>
+  <si>
+    <t>4.1.</t>
+  </si>
+  <si>
+    <t>4.2.</t>
+  </si>
+  <si>
+    <t>4.3.</t>
+  </si>
+  <si>
+    <t>5.1.</t>
+  </si>
+  <si>
+    <t>5.2.</t>
+  </si>
+  <si>
+    <t>5.3.</t>
+  </si>
+  <si>
+    <t>5.4.</t>
+  </si>
+  <si>
+    <t>5.5.</t>
+  </si>
+  <si>
+    <t>5.6.</t>
   </si>
 </sst>
 </file>
@@ -204,7 +303,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -329,11 +428,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -402,6 +512,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -702,8 +825,8 @@
   </sheetPr>
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1281,24 +1404,308 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="61.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="19" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A4" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="25.5">
+      <c r="A5" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="16"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="16"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="16"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A9" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="16"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="16"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A14" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="10"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="17"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="17"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A19" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" ht="25.5">
+      <c r="A21" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="17"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="17"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A25" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="22"/>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="1:4" ht="25.5">
+      <c r="A28" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="9"/>
+    </row>
+    <row r="31" spans="1:4" ht="25.5">
+      <c r="A31" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="9"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="18"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="11"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="96" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>